<commit_message>
partidos imagen y tooltips
</commit_message>
<xml_diff>
--- a/congresistasCuentasTwitter.xlsx
+++ b/congresistasCuentasTwitter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leibnitzpavel/Documents/GitHub/Congressman-Peru-Word-Cloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B31E8CC-664F-D744-A59B-5FA55F1823D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6621BEF0-B4C4-6348-BDEE-64580001CCB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="1415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="1421">
   <si>
     <t>partido</t>
   </si>
@@ -4280,6 +4280,24 @@
   </si>
   <si>
     <t>P13</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/8d/Logo_nuevo_peru.svg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/41/Peruanos_Por_el_Kambio.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/5/5a/Acci%C3%B3n_Republicana_de_Chile_2018.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/f/f2/Logo_Bancada_Liberal.jpg</t>
+  </si>
+  <si>
+    <t>https://previews.123rf.com/images/cd123/cd1231108/cd123110800011/10233390-empty-blank-emblem-badge-shield-logo-insignia-coat-of-arms.jpg</t>
+  </si>
+  <si>
+    <t>https://w1.buysub.com/pubs/SR/ADM/images/21_Circle_432_372.png</t>
   </si>
 </sst>
 </file>
@@ -21349,8 +21367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7AD9D7-3C0A-BC44-9946-396FBBD534FA}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21387,7 +21405,7 @@
         <v>1403</v>
       </c>
       <c r="B3" t="s">
-        <v>1389</v>
+        <v>1417</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>286</v>
@@ -21409,7 +21427,7 @@
         <v>1405</v>
       </c>
       <c r="B5" t="s">
-        <v>1391</v>
+        <v>1418</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>573</v>
@@ -21419,8 +21437,8 @@
       <c r="A6" t="s">
         <v>1406</v>
       </c>
-      <c r="B6" t="s">
-        <v>1392</v>
+      <c r="B6" s="10" t="s">
+        <v>1420</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>641</v>
@@ -21474,8 +21492,8 @@
       <c r="A11" t="s">
         <v>1411</v>
       </c>
-      <c r="B11" t="s">
-        <v>1400</v>
+      <c r="B11" s="10" t="s">
+        <v>1419</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>911</v>
@@ -21486,7 +21504,7 @@
         <v>1412</v>
       </c>
       <c r="B12" t="s">
-        <v>1397</v>
+        <v>1415</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1102</v>
@@ -21497,7 +21515,7 @@
         <v>1413</v>
       </c>
       <c r="B13" t="s">
-        <v>1398</v>
+        <v>1416</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1119</v>
@@ -21518,6 +21536,9 @@
       <c r="C15" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{7BBFFAA2-6AA7-0049-B6B2-ACAB4F45F4F1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>